<commit_message>
Added a new Test case
</commit_message>
<xml_diff>
--- a/src/testData/TestData.xlsx
+++ b/src/testData/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="38">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -118,6 +118,18 @@
   </si>
   <si>
     <t>Chrome</t>
+  </si>
+  <si>
+    <t>Framework_003</t>
+  </si>
+  <si>
+    <t>Framework_004</t>
+  </si>
+  <si>
+    <t>Pratik</t>
+  </si>
+  <si>
+    <t>29, LimeSquare, City Road</t>
   </si>
 </sst>
 </file>
@@ -516,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,7 +676,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
@@ -700,15 +712,56 @@
         <v>21</v>
       </c>
       <c r="M4" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M5" s="6" t="s">
         <v>23</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E5">
       <formula1>"Accessories, iMacs, iPads, iPhones"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F5">
       <formula1>"Product 1, Product 2, Product 3, Product 4"</formula1>
     </dataValidation>
   </dataValidations>
@@ -719,9 +772,11 @@
     <hyperlink ref="M3" r:id="rId4"/>
     <hyperlink ref="C4" r:id="rId5"/>
     <hyperlink ref="M4" r:id="rId6"/>
+    <hyperlink ref="C5" r:id="rId7"/>
+    <hyperlink ref="M5" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
changes made to framework
</commit_message>
<xml_diff>
--- a/src/testData/TestData.xlsx
+++ b/src/testData/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="41">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -136,12 +136,16 @@
   </si>
   <si>
     <t>Sourav</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -542,16 +546,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="17.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="4" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -637,6 +641,9 @@
       </c>
       <c r="M2" s="6" t="s">
         <v>23</v>
+      </c>
+      <c r="N2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
new test cases added to framework
</commit_message>
<xml_diff>
--- a/src/testData/TestData.xlsx
+++ b/src/testData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14190" windowHeight="1800" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14190" windowHeight="1800" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Register Account" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="108">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -308,6 +308,39 @@
   </si>
   <si>
     <t>test 11 (0),test 12 (0),test 20 (0),test 21 (0),test 15 (0),test 16 (0),test 17 (0),test 18 (0),test 19 (0),test 4 (0),test 5 (0),test 6 (0),test 7 (0),test 8 (0),test 9 (0),test 22 (0),test 23 (0),test 24 (0),Show All MP3 Players</t>
+  </si>
+  <si>
+    <t>TC20_fnCheck_LandingPage_SystemMenu_Tablets_Submenu_functionality</t>
+  </si>
+  <si>
+    <t>Tablets</t>
+  </si>
+  <si>
+    <t>TC21_fnCheck_LandingPage_SystemMenu_Software_Submenu_functionality</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>TC22_fnCheck_LandingPage_SystemMenu_PhonesandPDAs_Submenu_functionality</t>
+  </si>
+  <si>
+    <t>Phones &amp; PDAs</t>
+  </si>
+  <si>
+    <t>TC23_fnCheck_LandingPage_SystemMenu_Cameras_Submenu_functionality</t>
+  </si>
+  <si>
+    <t>Cameras</t>
+  </si>
+  <si>
+    <t>TC56_fnCheck_RegisterAccount_Page_Right_MenuBar_Elements</t>
+  </si>
+  <si>
+    <t>Login,Register,Forgotten Password,My Account,Address Book,Wish List,Order History,Downloads,Recurring payments,Recurring payments,Returns,Transactions,Newsletter</t>
+  </si>
+  <si>
+    <t>TC68_fnCheck_Login_Page_Right_MenuBar_Elements</t>
   </si>
 </sst>
 </file>
@@ -706,14 +739,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="74" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -956,9 +989,13 @@
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
+    <row r="31" spans="1:2" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>106</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -969,14 +1006,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="76.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1067,9 +1104,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
+    <row r="12" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
@@ -1195,10 +1236,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView topLeftCell="A16" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1335,6 +1376,38 @@
         <v>96</v>
       </c>
     </row>
+    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>